<commit_message>
Update Attendance Roster_Splunk Basic_October 16-17_.xlsx
</commit_message>
<xml_diff>
--- a/Attendance Roster_Splunk Basic_October 16-17_.xlsx
+++ b/Attendance Roster_Splunk Basic_October 16-17_.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VK_GIT\CISCO_SPLK_16_10_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7BDC7C-0E70-4140-8BCC-B8333C45736F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1951C2A0-6D7D-4701-8373-FDC34BF5DCD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="57">
   <si>
     <t>Start Date</t>
   </si>
@@ -191,13 +191,19 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>25MMS3001_U14</t>
+  </si>
+  <si>
+    <t>25MMS3001_U15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,6 +245,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -617,12 +635,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -634,9 +646,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -934,10 +954,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="24"/>
+      <c r="C1" s="30"/>
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1180,7 +1200,7 @@
   <dimension ref="B5:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1192,7 +1212,7 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="23" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1205,223 +1225,232 @@
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28" t="s">
+      <c r="D9" s="26"/>
+      <c r="E9" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="F9" s="26" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="27" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28" t="s">
+      <c r="D10" s="26"/>
+      <c r="E10" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="30" t="s">
+      <c r="F10" s="26" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="27" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28" t="s">
+      <c r="D11" s="26"/>
+      <c r="E11" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="26" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="27" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28" t="s">
+      <c r="D12" s="26"/>
+      <c r="E12" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="28" t="s">
+      <c r="F12" s="26" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28" t="s">
+      <c r="D13" s="26"/>
+      <c r="E13" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="F13" s="26" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="27" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28" t="s">
+      <c r="D14" s="26"/>
+      <c r="E14" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="28" t="s">
+      <c r="F14" s="26" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="27" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28" t="s">
+      <c r="D15" s="26"/>
+      <c r="E15" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="28" t="s">
+      <c r="F15" s="26" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="27" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28" t="s">
+      <c r="D16" s="26"/>
+      <c r="E16" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="28" t="s">
+      <c r="F16" s="26" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="27" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28" t="s">
+      <c r="D17" s="26"/>
+      <c r="E17" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="28" t="s">
+      <c r="F17" s="26" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="27" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28" t="s">
+      <c r="D18" s="26"/>
+      <c r="E18" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="F18" s="28" t="s">
+      <c r="F18" s="26" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="27" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28" t="s">
+      <c r="D19" s="26"/>
+      <c r="E19" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="F19" s="28" t="s">
+      <c r="F19" s="26" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="27" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28" t="s">
+      <c r="D20" s="26"/>
+      <c r="E20" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="F20" s="28" t="s">
+      <c r="F20" s="26" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="27" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="28"/>
-      <c r="E21" s="31" t="s">
+      <c r="D21" s="26"/>
+      <c r="E21" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="F21" s="30" t="s">
+      <c r="F21" s="26" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="29" t="s">
+    <row r="22" spans="2:6" ht="15" x14ac:dyDescent="0.3">
+      <c r="B22" s="27" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="29" t="s">
+      <c r="D22" s="26"/>
+      <c r="E22" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="15" x14ac:dyDescent="0.3">
+      <c r="B23" s="27" t="s">
         <v>18</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" location="/" display="https://cloud.cdp.rpsconsulting.in/console/ - /" xr:uid="{310FFD20-3796-4B0A-A8FB-29A6B991915D}"/>
   </hyperlinks>

</xml_diff>